<commit_message>
working branch for mac
</commit_message>
<xml_diff>
--- a/munsell_data/real_CIELAB.xlsx
+++ b/munsell_data/real_CIELAB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="Unspecified"/>
     </ext>
   </extLst>
 </workbook>
@@ -23,163 +23,163 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1638" uniqueCount="53">
   <si>
-    <t xml:space="preserve">file order</t>
+    <t>file order</t>
   </si>
   <si>
-    <t xml:space="preserve">h</t>
+    <t>h</t>
   </si>
   <si>
-    <t xml:space="preserve">V</t>
+    <t>V</t>
   </si>
   <si>
-    <t xml:space="preserve">C</t>
+    <t>C</t>
   </si>
   <si>
-    <t xml:space="preserve">x</t>
+    <t>x</t>
   </si>
   <si>
-    <t xml:space="preserve">y</t>
+    <t>y</t>
   </si>
   <si>
-    <t xml:space="preserve">Y</t>
+    <t>Y</t>
   </si>
   <si>
-    <t xml:space="preserve">X_C</t>
+    <t>X_C</t>
   </si>
   <si>
-    <t xml:space="preserve">Y_C</t>
+    <t>Y_C</t>
   </si>
   <si>
-    <t xml:space="preserve">Z_C</t>
+    <t>Z_C</t>
   </si>
   <si>
-    <t xml:space="preserve">L*</t>
+    <t>L*</t>
   </si>
   <si>
-    <t xml:space="preserve">a*</t>
+    <t>a*</t>
   </si>
   <si>
-    <t xml:space="preserve">b*</t>
+    <t>b*</t>
   </si>
   <si>
-    <t xml:space="preserve">10RP</t>
+    <t>10RP</t>
   </si>
   <si>
-    <t xml:space="preserve">2.5R</t>
+    <t>2.5R</t>
   </si>
   <si>
-    <t xml:space="preserve">5R</t>
+    <t>5R</t>
   </si>
   <si>
-    <t xml:space="preserve">7.5R</t>
+    <t>7.5R</t>
   </si>
   <si>
-    <t xml:space="preserve">10R</t>
+    <t>10R</t>
   </si>
   <si>
-    <t xml:space="preserve">2.5YR</t>
+    <t>2.5YR</t>
   </si>
   <si>
-    <t xml:space="preserve">5YR</t>
+    <t>5YR</t>
   </si>
   <si>
-    <t xml:space="preserve">7.5YR</t>
+    <t>7.5YR</t>
   </si>
   <si>
-    <t xml:space="preserve">10YR</t>
+    <t>10YR</t>
   </si>
   <si>
-    <t xml:space="preserve">2.5Y</t>
+    <t>2.5Y</t>
   </si>
   <si>
-    <t xml:space="preserve">5Y</t>
+    <t>5Y</t>
   </si>
   <si>
-    <t xml:space="preserve">7.5Y</t>
+    <t>7.5Y</t>
   </si>
   <si>
-    <t xml:space="preserve">10Y</t>
+    <t>10Y</t>
   </si>
   <si>
-    <t xml:space="preserve">2.5GY</t>
+    <t>2.5GY</t>
   </si>
   <si>
-    <t xml:space="preserve">5GY</t>
+    <t>5GY</t>
   </si>
   <si>
-    <t xml:space="preserve">7.5GY</t>
+    <t>7.5GY</t>
   </si>
   <si>
-    <t xml:space="preserve">10GY</t>
+    <t>10GY</t>
   </si>
   <si>
-    <t xml:space="preserve">2.5G</t>
+    <t>2.5G</t>
   </si>
   <si>
-    <t xml:space="preserve">5G</t>
+    <t>5G</t>
   </si>
   <si>
-    <t xml:space="preserve">7.5G</t>
+    <t>7.5G</t>
   </si>
   <si>
-    <t xml:space="preserve">10G</t>
+    <t>10G</t>
   </si>
   <si>
-    <t xml:space="preserve">2.5BG</t>
+    <t>2.5BG</t>
   </si>
   <si>
-    <t xml:space="preserve">5BG</t>
+    <t>5BG</t>
   </si>
   <si>
-    <t xml:space="preserve">7.5BG</t>
+    <t>7.5BG</t>
   </si>
   <si>
-    <t xml:space="preserve">10BG</t>
+    <t>10BG</t>
   </si>
   <si>
-    <t xml:space="preserve">2.5B</t>
+    <t>2.5B</t>
   </si>
   <si>
-    <t xml:space="preserve">5B</t>
+    <t>5B</t>
   </si>
   <si>
-    <t xml:space="preserve">7.5B</t>
+    <t>7.5B</t>
   </si>
   <si>
-    <t xml:space="preserve">10B</t>
+    <t>10B</t>
   </si>
   <si>
-    <t xml:space="preserve">2.5PB</t>
+    <t>2.5PB</t>
   </si>
   <si>
-    <t xml:space="preserve">5PB</t>
+    <t>5PB</t>
   </si>
   <si>
-    <t xml:space="preserve">7.5PB</t>
+    <t>7.5PB</t>
   </si>
   <si>
-    <t xml:space="preserve">10PB</t>
+    <t>10PB</t>
   </si>
   <si>
-    <t xml:space="preserve">2.5P</t>
+    <t>2.5P</t>
   </si>
   <si>
-    <t xml:space="preserve">5P</t>
+    <t>5P</t>
   </si>
   <si>
-    <t xml:space="preserve">7.5P</t>
+    <t>7.5P</t>
   </si>
   <si>
-    <t xml:space="preserve">10P</t>
+    <t>10P</t>
   </si>
   <si>
-    <t xml:space="preserve">2.5RP</t>
+    <t>2.5RP</t>
   </si>
   <si>
-    <t xml:space="preserve">5RP</t>
+    <t>5RP</t>
   </si>
   <si>
-    <t xml:space="preserve">7.5RP</t>
+    <t>7.5RP</t>
   </si>
 </sst>
 </file>
@@ -187,14 +187,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
-      <family val="0"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -214,13 +214,13 @@
     <font>
       <sz val="10"/>
       <name val="Courier New"/>
-      <family val="0"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
-      <family val="0"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -305,7 +305,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>369000</xdr:colOff>
+      <xdr:colOff>369360</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>38160</xdr:rowOff>
     </xdr:to>
@@ -317,34 +317,8 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="83520" y="63360"/>
-          <a:ext cx="8303400" cy="5587920"/>
+          <a:ext cx="8309520" cy="5587920"/>
         </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="21600" h="21600">
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="21600" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="21600" y="21600"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="21600"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="0"/>
-              </a:lnTo>
-              <a:close/>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
@@ -365,202 +339,217 @@
         <a:bodyPr lIns="27360" rIns="0" tIns="18000" bIns="0"/>
         <a:p>
           <a:r>
-            <a:rPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
+            <a:rPr lang="en-US" sz="1000" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Verdana"/>
             </a:rPr>
             <a:t>DISCLAIMER:</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
+          <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
+          <a:endParaRPr/>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
+            <a:rPr lang="en-US" sz="1000" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Verdana"/>
             </a:rPr>
             <a:t>These data are based on the Munsell Renotation data as found on the Munsel Color Science Laboratory web pages. Currently the path is here:</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
+          <a:endParaRPr/>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
+            <a:rPr lang="en-US" sz="1000" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Verdana"/>
             </a:rPr>
             <a:t>www.cis.rit.edu/research/mcsl/online/munsell.php</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
+          <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
+          <a:endParaRPr/>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
+            <a:rPr lang="en-US" sz="1000" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Verdana"/>
             </a:rPr>
             <a:t>The data file used here is real.dat. For details on the use of this file see the above web page.</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
+          <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
+          <a:endParaRPr/>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
+            <a:rPr lang="en-US" sz="1000" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Verdana"/>
             </a:rPr>
             <a:t>There are several additional columns of data in this file:</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
+          <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
+          <a:endParaRPr/>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
+            <a:rPr lang="en-US" sz="1000" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Verdana"/>
             </a:rPr>
             <a:t>file order - this is the row number of the data in real.dat</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
+          <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
+          <a:endParaRPr/>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
+            <a:rPr lang="en-US" sz="1000" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Verdana"/>
             </a:rPr>
             <a:t>HVC - Munsell notation (from real.dat)</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
+          <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
+          <a:endParaRPr/>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
+            <a:rPr lang="en-US" sz="1000" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Verdana"/>
             </a:rPr>
             <a:t>xyY - illuminant C chromaticity and luminance values (from real.dat)</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
+          <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
+          <a:endParaRPr/>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
+            <a:rPr lang="en-US" sz="1000" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Verdana"/>
             </a:rPr>
             <a:t>XYZ_C - illuminant C tristumulus values (traditional transform from xyY) (these are 2° 1931 based)</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
+          <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
+          <a:endParaRPr/>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
+            <a:rPr lang="en-US" sz="1000" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Verdana"/>
             </a:rPr>
             <a:t>CIELAB L* a* b* using illuminant C</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
+          <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
+          <a:endParaRPr/>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
+            <a:rPr lang="en-US" sz="1000" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Verdana"/>
             </a:rPr>
             <a:t>DRW 20Oct2011</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
+          <a:endParaRPr/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -576,14 +565,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.05"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="13"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -591,7 +577,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -607,14 +593,11 @@
   </sheetPr>
   <dimension ref="A1:M1626"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.05"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="13"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -67285,7 +67268,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>